<commit_message>
[Update] update create_map function
</commit_message>
<xml_diff>
--- a/simulation/python/Book1_copy_4.xlsx
+++ b/simulation/python/Book1_copy_4.xlsx
@@ -120,7 +120,7 @@
   <dimension ref="A1:E1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5859375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -164,7 +164,7 @@
         <v>240</v>
       </c>
       <c r="B3" s="0" t="n">
-        <v>185</v>
+        <v>220</v>
       </c>
       <c r="C3" s="0" t="n">
         <v>25</v>

</xml_diff>